<commit_message>
primer trimming using iVar + minor changes
</commit_message>
<xml_diff>
--- a/primer_schemes/DENGUESEQ1/V1/DENGUESEQ1.primers.xlsx
+++ b/primer_schemes/DENGUESEQ1/V1/DENGUESEQ1.primers.xlsx
@@ -2277,8 +2277,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100221A7C4456A97A45A5FB2F06EE0F3795" ma:contentTypeVersion="12" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="2f4c41121cfa066fe108e5e004855f00">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="56bd86cd-aee7-4d84-9328-0256d48ce484" xmlns:ns3="d89b8d59-050a-4503-a522-eb5bc4a69315" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6a311bf9b8bd512c3fc9f491e5d02bc" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100221A7C4456A97A45A5FB2F06EE0F3795" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="360c05c39a5b891b7d35833bebd587ce">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="56bd86cd-aee7-4d84-9328-0256d48ce484" xmlns:ns3="d89b8d59-050a-4503-a522-eb5bc4a69315" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b9a48877c9b5daa27d4eef0dcd4f5468" ns2:_="" ns3:_="">
     <xsd:import namespace="56bd86cd-aee7-4d84-9328-0256d48ce484"/>
     <xsd:import namespace="d89b8d59-050a-4503-a522-eb5bc4a69315"/>
     <xsd:element name="properties">
@@ -2318,7 +2318,7 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="11" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Marcações de imagem" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="143de60c-575b-4c62-9f62-591ff79d3e1c" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="11" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="143de60c-575b-4c62-9f62-591ff79d3e1c" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -2361,7 +2361,7 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d89b8d59-050a-4503-a522-eb5bc4a69315" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="18" nillable="true" ma:displayName="Compartilhado com" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="18" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -2380,7 +2380,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="19" nillable="true" ma:displayName="Detalhes de Compartilhado Com" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="19" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -2397,8 +2397,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de Conteúdo"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -2496,10 +2496,24 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="56bd86cd-aee7-4d84-9328-0256d48ce484">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6392EB6-0A47-4E10-843B-7F404730C175}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C971603-4DF7-41CB-BDC9-8D0265107F8B}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D77E376-DDC3-43DE-A33A-58A396DE6AD5}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9137918-7FFF-4099-B733-0443C005B40C}"/>
 </file>
</xml_diff>

<commit_message>
HIV-1 primer scheme (Sanabani et al. 2006)
</commit_message>
<xml_diff>
--- a/primer_schemes/DENGUESEQ1/V1/DENGUESEQ1.primers.xlsx
+++ b/primer_schemes/DENGUESEQ1/V1/DENGUESEQ1.primers.xlsx
@@ -2277,8 +2277,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100221A7C4456A97A45A5FB2F06EE0F3795" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="360c05c39a5b891b7d35833bebd587ce">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="56bd86cd-aee7-4d84-9328-0256d48ce484" xmlns:ns3="d89b8d59-050a-4503-a522-eb5bc4a69315" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b9a48877c9b5daa27d4eef0dcd4f5468" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100221A7C4456A97A45A5FB2F06EE0F3795" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4bd699d5528b09d9eaa63f72a227ae1d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="56bd86cd-aee7-4d84-9328-0256d48ce484" xmlns:ns3="d89b8d59-050a-4503-a522-eb5bc4a69315" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0bcf4575f77de29bfac727cc24d340ba" ns2:_="" ns3:_="">
     <xsd:import namespace="56bd86cd-aee7-4d84-9328-0256d48ce484"/>
     <xsd:import namespace="d89b8d59-050a-4503-a522-eb5bc4a69315"/>
     <xsd:element name="properties">
@@ -2298,6 +2298,7 @@
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -2355,6 +2356,11 @@
     <xsd:element name="MediaLengthInSeconds" ma:index="17" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="20" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -2507,7 +2513,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C971603-4DF7-41CB-BDC9-8D0265107F8B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{294D0FE2-898E-44EB-99B4-F1B3F4A33937}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>